<commit_message>
Curso Fundamentos sql server balta completo
</commit_message>
<xml_diff>
--- a/Desafio1/Sortear/Sortear/bin/Debug/net6.0-windows/Lista_de_funcionarios.xlsx
+++ b/Desafio1/Sortear/Sortear/bin/Debug/net6.0-windows/Lista_de_funcionarios.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <x:si>
     <x:t>Nome</x:t>
   </x:si>
@@ -66,7 +66,7 @@
     <x:t>Felipe Gabriel da Cunha</x:t>
   </x:si>
   <x:si>
-    <x:t>Felipe Rafael Tancredi Pascucci</x:t>
+    <x:t>Flavio Henrique Madureira Bergamini</x:t>
   </x:si>
   <x:si>
     <x:t>Gabriel Galhato Roriz</x:t>
@@ -75,6 +75,9 @@
     <x:t>Gabriel Junior de Souza</x:t>
   </x:si>
   <x:si>
+    <x:t>Gabriella da Silva Correia</x:t>
+  </x:si>
+  <x:si>
     <x:t>Giovanni Francez</x:t>
   </x:si>
   <x:si>
@@ -84,6 +87,9 @@
     <x:t>Guilherme Ribeiro de Melo Yabu</x:t>
   </x:si>
   <x:si>
+    <x:t>Guilherme Soares Battaglin</x:t>
+  </x:si>
+  <x:si>
     <x:t>Gustavo de Paiva Caiafa</x:t>
   </x:si>
   <x:si>
@@ -118,9 +124,6 @@
   </x:si>
   <x:si>
     <x:t>Lucas Thalles dos Santos</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Marcelo Bruno Verissimo Mendes Moraes Viegas</x:t>
   </x:si>
   <x:si>
     <x:t>Matheus Cleber Silva Guerra</x:t>
@@ -880,7 +883,9 @@
       </x:c>
     </x:row>
     <x:row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <x:c r="A54" s="2" t="s"/>
+      <x:c r="A54" s="2" t="s">
+        <x:v>53</x:v>
+      </x:c>
     </x:row>
     <x:row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <x:c r="A55" s="4" t="s"/>

</xml_diff>